<commit_message>
Regretion Run SCD0034 - Hak Akses Report Pencapaian Booster, SCD0035 - Akses Pencapaian Booster, SCD0036 - Akses Pencapaian Booster, SCD0037 - Akses Pencapaian Booster, and SCD0038 - Akses Pencapaian Booster
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0035_Hak Akses Report Pencapaian Booster.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0035_Hak Akses Report Pencapaian Booster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0539E80-11CC-4DFC-AA77-A1338CA11B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8A1EFA-8209-462C-8ECA-EF3043D60288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0035" sheetId="2" r:id="rId1"/>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -246,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,9 +582,10 @@
     <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" customWidth="1"/>
     <col min="18" max="18" width="30.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.140625" customWidth="1"/>
+    <col min="20" max="20" width="26" customWidth="1"/>
     <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -661,7 +665,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="390" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="225" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -718,10 +722,10 @@
       <c r="T2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="16" t="s">
         <v>37</v>
       </c>
       <c r="Y2" t="s">

</xml_diff>